<commit_message>
Update task1 and task 2.
</commit_message>
<xml_diff>
--- a/FreeNow_Task2_SoftwareRelease.xlsx
+++ b/FreeNow_Task2_SoftwareRelease.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehedizamanhimel/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehedizamanhimel/Documents/FreeNowApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63CC34D-2509-EF46-8830-433476B20A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD4ED95-5AB1-1949-8F89-75990019870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="880" windowWidth="17060" windowHeight="21540" xr2:uid="{C5C45E9E-7B5B-2043-8B6F-4DCDA620412F}"/>
+    <workbookView xWindow="12760" yWindow="-21100" windowWidth="23560" windowHeight="19880" xr2:uid="{C5C45E9E-7B5B-2043-8B6F-4DCDA620412F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Verifying chat hisory</t>
   </si>
   <si>
-    <t>Sign in</t>
-  </si>
-  <si>
     <t>Logout</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Permission check for internal storage (Gallery, File explorer, Contact list)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sending/ Receive data. </t>
-  </si>
-  <si>
     <t>Sending initially on offline, then try sending with internet.</t>
   </si>
   <si>
@@ -67,18 +61,62 @@
     <t>Test Cases</t>
   </si>
   <si>
-    <t>Test Steps</t>
-  </si>
-  <si>
-    <t>Running Smoke Test</t>
+    <t>Profile update</t>
+  </si>
+  <si>
+    <t>Sending a message</t>
+  </si>
+  <si>
+    <t>Receiving a message</t>
+  </si>
+  <si>
+    <t>Login via QR code</t>
+  </si>
+  <si>
+    <t>Regular Login</t>
+  </si>
+  <si>
+    <t>Viewing chatbox with particular user details</t>
+  </si>
+  <si>
+    <t>Opening of app (internet on and cache mode)</t>
+  </si>
+  <si>
+    <t>Checking input methods (Keyboard, Mic)</t>
+  </si>
+  <si>
+    <t>Verifying that push notificatons are woring properly with and without permission.</t>
+  </si>
+  <si>
+    <t>Running Automated Smoke Test</t>
+  </si>
+  <si>
+    <t>Feature Testing (Automated or Manual)</t>
+  </si>
+  <si>
+    <t>Checking the web version with different browsers</t>
+  </si>
+  <si>
+    <t>New contact syncing</t>
+  </si>
+  <si>
+    <t>App background and forground working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,10 +144,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,10 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485263F2-4F1B-E343-BD5B-326C2E38BD6B}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,61 +487,131 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Sensitivity: Internal</oddFooter>

</xml_diff>